<commit_message>
translate glossary of laws in italian
</commit_message>
<xml_diff>
--- a/it/data_and_scripts/data/datasetLaws.xlsx
+++ b/it/data_and_scripts/data/datasetLaws.xlsx
@@ -1,28 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitch/Google Drive/Work/Assegno di Ricerca 2017_2018/[2017-09] SIEC - History of Administrative Detention/1. Material/Resources/Corrected Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amelia/Documents/GitHub/00_work/prototype-siec/it/data_and_scripts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57FC1A5-15E2-D648-96B7-CA69BA62F5A9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="17840" tabRatio="871"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28780" windowHeight="19520" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all law" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'all law'!$A$1:$H$339</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'all law'!$A$1:$I$358</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="179017" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2001" uniqueCount="1072">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2009" uniqueCount="1076">
   <si>
     <t>AG001</t>
   </si>
@@ -3238,12 +3240,24 @@
   </si>
   <si>
     <t>intercantonal</t>
+  </si>
+  <si>
+    <t>cantonale</t>
+  </si>
+  <si>
+    <t>federale</t>
+  </si>
+  <si>
+    <t>intercantonale</t>
+  </si>
+  <si>
+    <t>internazionale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -3358,7 +3372,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Excel Built-in Normal" xfId="1"/>
+    <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3755,11 +3769,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IO358"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:IN358"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A354" workbookViewId="0">
-      <selection activeCell="C367" sqref="C367"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3769,7 +3783,7 @@
     <col min="4" max="5" width="11.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="24.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="2" customWidth="1"/>
-    <col min="8" max="249" width="11.6640625" style="1" customWidth="1"/>
+    <col min="8" max="248" width="11.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23" customHeight="1" x14ac:dyDescent="0.2">
@@ -3821,7 +3835,7 @@
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -3841,7 +3855,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -3864,7 +3878,7 @@
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -3887,7 +3901,7 @@
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -3912,7 +3926,7 @@
         <v>17</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -3937,7 +3951,7 @@
         <v>20</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -3962,7 +3976,7 @@
         <v>23</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -3987,7 +4001,7 @@
         <v>27</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -4012,7 +4026,7 @@
         <v>31</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -4032,7 +4046,7 @@
         <v>35</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="37.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4055,7 +4069,7 @@
         <v>31</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4078,7 +4092,7 @@
         <v>42</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4101,7 +4115,7 @@
         <v>46</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4121,7 +4135,7 @@
         <v>50</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4141,7 +4155,7 @@
         <v>3</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -4164,7 +4178,7 @@
         <v>55</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4187,7 +4201,7 @@
         <v>58</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4207,7 +4221,7 @@
         <v>3</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4230,7 +4244,7 @@
         <v>31</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4250,7 +4264,7 @@
         <v>2</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -4270,7 +4284,7 @@
         <v>4</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -4290,7 +4304,7 @@
         <v>2</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="118" x14ac:dyDescent="0.2">
@@ -4310,7 +4324,7 @@
         <v>13</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4330,7 +4344,7 @@
         <v>50</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4350,7 +4364,7 @@
         <v>1</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4370,7 +4384,7 @@
         <v>1</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4390,7 +4404,7 @@
         <v>35</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -4410,7 +4424,7 @@
         <v>2</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -4430,7 +4444,7 @@
         <v>83</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4450,7 +4464,7 @@
         <v>35</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4470,7 +4484,7 @@
         <v>35</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4490,7 +4504,7 @@
         <v>35</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4510,7 +4524,7 @@
         <v>13</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4530,7 +4544,7 @@
         <v>35</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4550,7 +4564,7 @@
         <v>2</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -4570,7 +4584,7 @@
         <v>4</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4593,7 +4607,7 @@
       </c>
       <c r="H38" s="13"/>
       <c r="I38" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="118" x14ac:dyDescent="0.2">
@@ -4616,7 +4630,7 @@
       </c>
       <c r="H39" s="13"/>
       <c r="I39" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -4639,7 +4653,7 @@
       </c>
       <c r="H40" s="13"/>
       <c r="I40" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -4662,7 +4676,7 @@
       </c>
       <c r="H41" s="13"/>
       <c r="I41" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -4685,7 +4699,7 @@
       </c>
       <c r="H42" s="13"/>
       <c r="I42" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -4708,7 +4722,7 @@
       </c>
       <c r="H43" s="13"/>
       <c r="I43" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -4731,7 +4745,7 @@
       </c>
       <c r="H44" s="13"/>
       <c r="I44" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4754,7 +4768,7 @@
       </c>
       <c r="H45" s="13"/>
       <c r="I45" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="118" x14ac:dyDescent="0.2">
@@ -4775,7 +4789,7 @@
       </c>
       <c r="H46" s="13"/>
       <c r="I46" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -4796,7 +4810,7 @@
       </c>
       <c r="H47" s="13"/>
       <c r="I47" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="118" x14ac:dyDescent="0.2">
@@ -4817,7 +4831,7 @@
       </c>
       <c r="H48" s="13"/>
       <c r="I48" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="144" x14ac:dyDescent="0.2">
@@ -4838,7 +4852,7 @@
       </c>
       <c r="H49" s="13"/>
       <c r="I49" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -4859,7 +4873,7 @@
       </c>
       <c r="H50" s="13"/>
       <c r="I50" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4881,7 +4895,7 @@
         <v>83</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -4903,7 +4917,7 @@
         <v>35</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -4925,7 +4939,7 @@
         <v>83</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -4947,7 +4961,7 @@
         <v>83</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4969,7 +4983,7 @@
         <v>83</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -4991,7 +5005,7 @@
         <v>83</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5013,7 +5027,7 @@
         <v>83</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5040,7 +5054,7 @@
         <v>27</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -5063,7 +5077,7 @@
       </c>
       <c r="H59" s="8"/>
       <c r="I59" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -5086,7 +5100,7 @@
       </c>
       <c r="H60" s="8"/>
       <c r="I60" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -5109,7 +5123,7 @@
       </c>
       <c r="H61" s="8"/>
       <c r="I61" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -5136,7 +5150,7 @@
         <v>177</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="118" x14ac:dyDescent="0.2">
@@ -5159,7 +5173,7 @@
       </c>
       <c r="H63" s="5"/>
       <c r="I63" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -5184,7 +5198,7 @@
       </c>
       <c r="H64" s="5"/>
       <c r="I64" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5209,7 +5223,7 @@
         <v>185</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -5232,7 +5246,7 @@
       </c>
       <c r="H66" s="5"/>
       <c r="I66" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5257,7 +5271,7 @@
         <v>191</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -5280,7 +5294,7 @@
       </c>
       <c r="H68" s="5"/>
       <c r="I68" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -5305,7 +5319,7 @@
         <v>197</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -5328,7 +5342,7 @@
       </c>
       <c r="H70" s="5"/>
       <c r="I70" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -5353,7 +5367,7 @@
         <v>204</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -5376,7 +5390,7 @@
       </c>
       <c r="H72" s="5"/>
       <c r="I72" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5399,7 +5413,7 @@
         <v>209</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5420,7 +5434,7 @@
       </c>
       <c r="H74" s="13"/>
       <c r="I74" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -5441,7 +5455,7 @@
       </c>
       <c r="H75" s="13"/>
       <c r="I75" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -5464,7 +5478,7 @@
         <v>216</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -5485,7 +5499,7 @@
       </c>
       <c r="H77" s="13"/>
       <c r="I77" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -5508,7 +5522,7 @@
         <v>221</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -5531,7 +5545,7 @@
         <v>224</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -5552,7 +5566,7 @@
       </c>
       <c r="H80" s="13"/>
       <c r="I80" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -5575,7 +5589,7 @@
       </c>
       <c r="H81" s="3"/>
       <c r="I81" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5598,7 +5612,7 @@
       </c>
       <c r="H82" s="3"/>
       <c r="I82" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -5623,7 +5637,7 @@
         <v>237</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5648,7 +5662,7 @@
         <v>241</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -5673,7 +5687,7 @@
         <v>245</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -5698,7 +5712,7 @@
         <v>248</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -5723,7 +5737,7 @@
         <v>252</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -5748,7 +5762,7 @@
         <v>255</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -5773,7 +5787,7 @@
         <v>259</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="118" x14ac:dyDescent="0.2">
@@ -5798,7 +5812,7 @@
         <v>263</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5821,7 +5835,7 @@
       </c>
       <c r="H91" s="5"/>
       <c r="I91" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -5844,7 +5858,7 @@
       </c>
       <c r="H92" s="5"/>
       <c r="I92" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -5869,7 +5883,7 @@
         <v>273</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -5889,7 +5903,7 @@
         <v>4</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5911,7 +5925,7 @@
         <v>83</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -5933,7 +5947,7 @@
         <v>83</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -5955,7 +5969,7 @@
         <v>35</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5977,7 +5991,7 @@
         <v>83</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -5999,7 +6013,7 @@
         <v>83</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6021,7 +6035,7 @@
         <v>83</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -6043,7 +6057,7 @@
         <v>35</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6065,7 +6079,7 @@
         <v>13</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6087,7 +6101,7 @@
         <v>13</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6109,7 +6123,7 @@
         <v>35</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6131,7 +6145,7 @@
         <v>83</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6151,7 +6165,7 @@
         <v>1</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6171,7 +6185,7 @@
         <v>1</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -6194,7 +6208,7 @@
       </c>
       <c r="H108" s="3"/>
       <c r="I108" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6219,7 +6233,7 @@
         <v>323</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="110" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6242,7 +6256,7 @@
       </c>
       <c r="H110" s="8"/>
       <c r="I110" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6267,7 +6281,7 @@
         <v>330</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="112" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6292,7 +6306,7 @@
         <v>334</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -6317,7 +6331,7 @@
         <v>338</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6340,7 +6354,7 @@
       </c>
       <c r="H114" s="5"/>
       <c r="I114" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6363,7 +6377,7 @@
       </c>
       <c r="H115" s="5"/>
       <c r="I115" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6386,7 +6400,7 @@
       </c>
       <c r="H116" s="5"/>
       <c r="I116" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6411,7 +6425,7 @@
         <v>351</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -6434,7 +6448,7 @@
       </c>
       <c r="H118" s="5"/>
       <c r="I118" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -6459,7 +6473,7 @@
         <v>358</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6484,7 +6498,7 @@
         <v>362</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="121" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6507,7 +6521,7 @@
       </c>
       <c r="H121" s="5"/>
       <c r="I121" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="122" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -6532,7 +6546,7 @@
         <v>368</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6557,7 +6571,7 @@
         <v>371</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="124" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -6580,7 +6594,7 @@
       </c>
       <c r="H124" s="5"/>
       <c r="I124" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="125" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6605,7 +6619,7 @@
         <v>376</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6630,7 +6644,7 @@
         <v>379</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6655,7 +6669,7 @@
         <v>382</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -6680,7 +6694,7 @@
         <v>385</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="129" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6705,7 +6719,7 @@
         <v>388</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -6728,7 +6742,7 @@
       </c>
       <c r="H130" s="5"/>
       <c r="I130" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6753,7 +6767,7 @@
         <v>393</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -6778,7 +6792,7 @@
         <v>396</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6803,7 +6817,7 @@
         <v>399</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6826,7 +6840,7 @@
       </c>
       <c r="H134" s="8"/>
       <c r="I134" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -6849,7 +6863,7 @@
       </c>
       <c r="H135" s="5"/>
       <c r="I135" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -6872,7 +6886,7 @@
       </c>
       <c r="H136" s="8"/>
       <c r="I136" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.2">
@@ -6895,7 +6909,7 @@
       </c>
       <c r="H137" s="5"/>
       <c r="I137" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -6918,7 +6932,7 @@
       </c>
       <c r="H138" s="5"/>
       <c r="I138" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="139" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -6941,7 +6955,7 @@
       </c>
       <c r="H139" s="5"/>
       <c r="I139" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="140" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -6964,7 +6978,7 @@
       </c>
       <c r="H140" s="8"/>
       <c r="I140" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="141" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -6987,7 +7001,7 @@
       </c>
       <c r="H141" s="8"/>
       <c r="I141" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="142" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7010,7 +7024,7 @@
       </c>
       <c r="H142" s="8"/>
       <c r="I142" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="143" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -7033,7 +7047,7 @@
       </c>
       <c r="H143" s="8"/>
       <c r="I143" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="144" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7056,7 +7070,7 @@
       </c>
       <c r="H144" s="8"/>
       <c r="I144" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="145" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -7079,7 +7093,7 @@
       </c>
       <c r="H145" s="8"/>
       <c r="I145" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="146" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -7102,7 +7116,7 @@
       </c>
       <c r="H146" s="5"/>
       <c r="I146" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="147" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -7125,7 +7139,7 @@
       </c>
       <c r="H147" s="5"/>
       <c r="I147" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="148" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -7148,7 +7162,7 @@
       </c>
       <c r="H148" s="5"/>
       <c r="I148" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="149" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -7171,7 +7185,7 @@
       </c>
       <c r="H149" s="5"/>
       <c r="I149" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="150" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -7196,7 +7210,7 @@
         <v>454</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="151" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -7221,7 +7235,7 @@
         <v>458</v>
       </c>
       <c r="I151" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="152" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7244,7 +7258,7 @@
       </c>
       <c r="H152" s="5"/>
       <c r="I152" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="153" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -7269,7 +7283,7 @@
         <v>465</v>
       </c>
       <c r="I153" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="154" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -7292,7 +7306,7 @@
       </c>
       <c r="H154" s="5"/>
       <c r="I154" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="155" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -7315,7 +7329,7 @@
       </c>
       <c r="H155" s="5"/>
       <c r="I155" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="156" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -7338,7 +7352,7 @@
       </c>
       <c r="H156" s="5"/>
       <c r="I156" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="157" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -7361,7 +7375,7 @@
       </c>
       <c r="H157" s="5"/>
       <c r="I157" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="158" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -7388,7 +7402,7 @@
         <v>482</v>
       </c>
       <c r="I158" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="159" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -7413,7 +7427,7 @@
         <v>486</v>
       </c>
       <c r="I159" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -7436,7 +7450,7 @@
       </c>
       <c r="H160" s="5"/>
       <c r="I160" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="161" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -7459,7 +7473,7 @@
       </c>
       <c r="H161" s="5"/>
       <c r="I161" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="162" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -7482,7 +7496,7 @@
       </c>
       <c r="H162" s="5"/>
       <c r="I162" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -7505,7 +7519,7 @@
       </c>
       <c r="H163" s="5"/>
       <c r="I163" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="164" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7530,7 +7544,7 @@
         <v>496</v>
       </c>
       <c r="I164" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="165" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -7553,7 +7567,7 @@
       </c>
       <c r="H165" s="3"/>
       <c r="I165" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="166" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -7576,7 +7590,7 @@
       </c>
       <c r="H166" s="5"/>
       <c r="I166" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="167" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7599,7 +7613,7 @@
       </c>
       <c r="H167" s="5"/>
       <c r="I167" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="168" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7622,7 +7636,7 @@
       </c>
       <c r="H168" s="5"/>
       <c r="I168" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="169" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7645,7 +7659,7 @@
       </c>
       <c r="H169" s="5"/>
       <c r="I169" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="170" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7668,7 +7682,7 @@
       </c>
       <c r="H170" s="13"/>
       <c r="I170" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="171" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -7691,7 +7705,7 @@
       </c>
       <c r="H171" s="13"/>
       <c r="I171" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="172" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -7714,7 +7728,7 @@
       </c>
       <c r="H172" s="13"/>
       <c r="I172" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -7736,7 +7750,7 @@
         <v>1</v>
       </c>
       <c r="I173" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="174" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -7759,7 +7773,7 @@
       </c>
       <c r="H174" s="8"/>
       <c r="I174" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="175" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -7782,7 +7796,7 @@
       </c>
       <c r="H175" s="5"/>
       <c r="I175" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="176" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -7805,7 +7819,7 @@
       </c>
       <c r="H176" s="5"/>
       <c r="I176" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="177" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7828,7 +7842,7 @@
       </c>
       <c r="H177" s="5"/>
       <c r="I177" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="178" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -7851,7 +7865,7 @@
       </c>
       <c r="H178" s="5"/>
       <c r="I178" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="179" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -7874,7 +7888,7 @@
       </c>
       <c r="H179" s="8"/>
       <c r="I179" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="180" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -7897,7 +7911,7 @@
       </c>
       <c r="H180" s="8"/>
       <c r="I180" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="181" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7920,7 +7934,7 @@
       </c>
       <c r="H181" s="8"/>
       <c r="I181" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="182" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7943,7 +7957,7 @@
       </c>
       <c r="H182" s="5"/>
       <c r="I182" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="183" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -7966,7 +7980,7 @@
       </c>
       <c r="H183" s="5"/>
       <c r="I183" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="184" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -7989,7 +8003,7 @@
       </c>
       <c r="H184" s="5"/>
       <c r="I184" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="185" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8012,7 +8026,7 @@
       </c>
       <c r="H185" s="5"/>
       <c r="I185" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="186" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8035,7 +8049,7 @@
       </c>
       <c r="H186" s="5"/>
       <c r="I186" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="187" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8058,7 +8072,7 @@
       </c>
       <c r="H187" s="5"/>
       <c r="I187" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="188" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8081,7 +8095,7 @@
       </c>
       <c r="H188" s="8"/>
       <c r="I188" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="189" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8104,7 +8118,7 @@
       </c>
       <c r="H189" s="8"/>
       <c r="I189" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="190" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -8127,7 +8141,7 @@
       </c>
       <c r="H190" s="5"/>
       <c r="I190" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="191" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8150,7 +8164,7 @@
       </c>
       <c r="H191" s="5"/>
       <c r="I191" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="192" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8173,7 +8187,7 @@
       </c>
       <c r="H192" s="5"/>
       <c r="I192" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="193" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -8196,7 +8210,7 @@
       </c>
       <c r="H193" s="5"/>
       <c r="I193" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="194" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -8219,7 +8233,7 @@
       </c>
       <c r="H194" s="5"/>
       <c r="I194" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="195" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8242,7 +8256,7 @@
       </c>
       <c r="H195" s="5"/>
       <c r="I195" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="196" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8265,7 +8279,7 @@
       </c>
       <c r="H196" s="13"/>
       <c r="I196" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="197" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8288,7 +8302,7 @@
       </c>
       <c r="H197" s="13"/>
       <c r="I197" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="198" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8311,7 +8325,7 @@
       </c>
       <c r="H198" s="13"/>
       <c r="I198" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="199" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -8334,7 +8348,7 @@
       </c>
       <c r="H199" s="13"/>
       <c r="I199" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="200" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -8357,7 +8371,7 @@
       </c>
       <c r="H200" s="13"/>
       <c r="I200" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="201" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8380,7 +8394,7 @@
       </c>
       <c r="H201" s="13"/>
       <c r="I201" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="202" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8403,7 +8417,7 @@
       </c>
       <c r="H202" s="13"/>
       <c r="I202" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="203" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8426,7 +8440,7 @@
       </c>
       <c r="H203" s="13"/>
       <c r="I203" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="204" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -8449,7 +8463,7 @@
       </c>
       <c r="H204" s="13"/>
       <c r="I204" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="205" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -8472,7 +8486,7 @@
       </c>
       <c r="H205" s="13"/>
       <c r="I205" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="206" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -8495,7 +8509,7 @@
       </c>
       <c r="H206" s="13"/>
       <c r="I206" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="207" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8518,7 +8532,7 @@
       </c>
       <c r="H207" s="13"/>
       <c r="I207" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="208" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8541,7 +8555,7 @@
       </c>
       <c r="H208" s="13"/>
       <c r="I208" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="209" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -8564,7 +8578,7 @@
       </c>
       <c r="H209" s="13"/>
       <c r="I209" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="210" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8587,7 +8601,7 @@
       </c>
       <c r="H210" s="13"/>
       <c r="I210" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="211" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -8610,7 +8624,7 @@
       </c>
       <c r="H211" s="13"/>
       <c r="I211" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="212" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8633,7 +8647,7 @@
       </c>
       <c r="H212" s="13"/>
       <c r="I212" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="213" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8656,7 +8670,7 @@
       </c>
       <c r="H213" s="8"/>
       <c r="I213" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="214" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8679,7 +8693,7 @@
       </c>
       <c r="H214" s="8"/>
       <c r="I214" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="215" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8702,7 +8716,7 @@
       </c>
       <c r="H215" s="8"/>
       <c r="I215" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="216" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -8725,7 +8739,7 @@
       </c>
       <c r="H216" s="5"/>
       <c r="I216" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="217" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8748,7 +8762,7 @@
       </c>
       <c r="H217" s="5"/>
       <c r="I217" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="218" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -8771,7 +8785,7 @@
       </c>
       <c r="H218" s="5"/>
       <c r="I218" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="219" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8794,7 +8808,7 @@
       </c>
       <c r="H219" s="5"/>
       <c r="I219" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="220" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8817,7 +8831,7 @@
       </c>
       <c r="H220" s="8"/>
       <c r="I220" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="221" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8840,7 +8854,7 @@
       </c>
       <c r="H221" s="8"/>
       <c r="I221" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="222" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -8863,7 +8877,7 @@
       </c>
       <c r="H222" s="5"/>
       <c r="I222" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="223" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -8888,7 +8902,7 @@
       </c>
       <c r="H223" s="5"/>
       <c r="I223" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="224" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -8911,7 +8925,7 @@
       </c>
       <c r="H224" s="5"/>
       <c r="I224" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="225" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8936,7 +8950,7 @@
       </c>
       <c r="H225" s="5"/>
       <c r="I225" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="226" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8961,7 +8975,7 @@
       </c>
       <c r="H226" s="5"/>
       <c r="I226" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="227" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -8984,7 +8998,7 @@
       </c>
       <c r="H227" s="5"/>
       <c r="I227" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="228" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -9009,7 +9023,7 @@
       </c>
       <c r="H228" s="5"/>
       <c r="I228" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="229" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -9032,7 +9046,7 @@
       </c>
       <c r="H229" s="5"/>
       <c r="I229" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="230" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -9057,7 +9071,7 @@
       </c>
       <c r="H230" s="5"/>
       <c r="I230" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="231" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -9080,7 +9094,7 @@
       </c>
       <c r="H231" s="5"/>
       <c r="I231" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="232" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -9103,7 +9117,7 @@
       </c>
       <c r="H232" s="5"/>
       <c r="I232" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="233" spans="1:9" ht="118" x14ac:dyDescent="0.2">
@@ -9128,7 +9142,7 @@
       </c>
       <c r="H233" s="5"/>
       <c r="I233" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="234" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -9151,7 +9165,7 @@
       </c>
       <c r="H234" s="5"/>
       <c r="I234" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="235" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -9174,7 +9188,7 @@
       </c>
       <c r="H235" s="5"/>
       <c r="I235" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="236" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -9199,7 +9213,7 @@
       </c>
       <c r="H236" s="5"/>
       <c r="I236" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="237" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -9222,7 +9236,7 @@
       </c>
       <c r="H237" s="5"/>
       <c r="I237" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="238" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -9245,7 +9259,7 @@
       </c>
       <c r="H238" s="5"/>
       <c r="I238" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="239" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -9265,7 +9279,7 @@
         <v>1</v>
       </c>
       <c r="I239" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="240" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -9288,7 +9302,7 @@
       </c>
       <c r="H240" s="13"/>
       <c r="I240" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="241" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -9311,7 +9325,7 @@
       </c>
       <c r="H241" s="13"/>
       <c r="I241" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="242" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -9334,7 +9348,7 @@
       </c>
       <c r="H242" s="8"/>
       <c r="I242" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="243" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -9357,7 +9371,7 @@
       </c>
       <c r="H243" s="5"/>
       <c r="I243" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="244" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -9380,7 +9394,7 @@
       </c>
       <c r="H244" s="5"/>
       <c r="I244" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="245" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -9403,7 +9417,7 @@
       </c>
       <c r="H245" s="5"/>
       <c r="I245" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="246" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -9426,7 +9440,7 @@
       </c>
       <c r="H246" s="5"/>
       <c r="I246" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="247" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -9449,7 +9463,7 @@
       </c>
       <c r="H247" s="5"/>
       <c r="I247" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="248" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -9472,7 +9486,7 @@
       </c>
       <c r="H248" s="5"/>
       <c r="I248" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="249" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -9495,7 +9509,7 @@
       </c>
       <c r="H249" s="5"/>
       <c r="I249" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="250" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -9518,7 +9532,7 @@
       </c>
       <c r="H250" s="5"/>
       <c r="I250" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="251" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -9541,7 +9555,7 @@
       </c>
       <c r="H251" s="5"/>
       <c r="I251" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="252" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -9564,7 +9578,7 @@
       </c>
       <c r="H252" s="5"/>
       <c r="I252" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="253" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -9587,7 +9601,7 @@
       </c>
       <c r="H253" s="5"/>
       <c r="I253" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="254" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -9610,7 +9624,7 @@
       </c>
       <c r="H254" s="5"/>
       <c r="I254" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="255" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -9633,7 +9647,7 @@
       </c>
       <c r="H255" s="5"/>
       <c r="I255" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="256" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -9656,7 +9670,7 @@
       </c>
       <c r="H256" s="5"/>
       <c r="I256" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="257" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -9679,7 +9693,7 @@
       </c>
       <c r="H257" s="5"/>
       <c r="I257" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="258" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -9699,7 +9713,7 @@
         <v>2</v>
       </c>
       <c r="I258" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="259" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -9722,7 +9736,7 @@
       </c>
       <c r="H259" s="5"/>
       <c r="I259" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="260" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -9745,7 +9759,7 @@
       </c>
       <c r="H260" s="5"/>
       <c r="I260" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="261" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -9768,7 +9782,7 @@
       </c>
       <c r="H261" s="5"/>
       <c r="I261" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="262" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -9793,7 +9807,7 @@
         <v>351</v>
       </c>
       <c r="I262" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="263" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -9818,7 +9832,7 @@
         <v>783</v>
       </c>
       <c r="I263" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="264" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -9843,7 +9857,7 @@
         <v>787</v>
       </c>
       <c r="I264" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="265" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -9866,7 +9880,7 @@
       </c>
       <c r="H265" s="5"/>
       <c r="I265" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="266" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -9889,7 +9903,7 @@
       </c>
       <c r="H266" s="5"/>
       <c r="I266" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="267" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -9912,7 +9926,7 @@
       </c>
       <c r="H267" s="5"/>
       <c r="I267" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="268" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -9937,7 +9951,7 @@
         <v>351</v>
       </c>
       <c r="I268" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="269" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -9962,7 +9976,7 @@
         <v>221</v>
       </c>
       <c r="I269" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="270" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -9987,7 +10001,7 @@
         <v>23</v>
       </c>
       <c r="I270" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="271" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -10012,7 +10026,7 @@
         <v>803</v>
       </c>
       <c r="I271" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="272" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -10037,7 +10051,7 @@
         <v>806</v>
       </c>
       <c r="I272" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="273" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -10060,7 +10074,7 @@
       </c>
       <c r="H273" s="5"/>
       <c r="I273" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="274" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -10083,7 +10097,7 @@
       </c>
       <c r="H274" s="3"/>
       <c r="I274" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="275" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -10106,7 +10120,7 @@
       </c>
       <c r="H275" s="3"/>
       <c r="I275" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="276" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -10129,7 +10143,7 @@
       </c>
       <c r="H276" s="3"/>
       <c r="I276" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="277" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -10152,7 +10166,7 @@
       </c>
       <c r="H277" s="8"/>
       <c r="I277" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="278" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -10175,7 +10189,7 @@
       </c>
       <c r="H278" s="5"/>
       <c r="I278" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="279" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -10198,7 +10212,7 @@
       </c>
       <c r="H279" s="5"/>
       <c r="I279" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="280" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -10221,7 +10235,7 @@
       </c>
       <c r="H280" s="5"/>
       <c r="I280" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="281" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -10244,7 +10258,7 @@
       </c>
       <c r="H281" s="5"/>
       <c r="I281" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="282" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -10267,7 +10281,7 @@
       </c>
       <c r="H282" s="5"/>
       <c r="I282" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="283" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -10290,7 +10304,7 @@
       </c>
       <c r="H283" s="5"/>
       <c r="I283" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="284" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -10313,7 +10327,7 @@
       </c>
       <c r="H284" s="5"/>
       <c r="I284" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="285" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -10333,7 +10347,7 @@
         <v>203</v>
       </c>
       <c r="I285" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="286" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -10356,7 +10370,7 @@
       </c>
       <c r="H286" s="8"/>
       <c r="I286" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="287" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -10379,7 +10393,7 @@
       </c>
       <c r="H287" s="8"/>
       <c r="I287" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="288" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -10402,7 +10416,7 @@
       </c>
       <c r="H288" s="8"/>
       <c r="I288" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="289" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -10425,7 +10439,7 @@
       </c>
       <c r="H289" s="5"/>
       <c r="I289" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="290" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -10448,7 +10462,7 @@
       </c>
       <c r="H290" s="8"/>
       <c r="I290" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="291" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -10471,7 +10485,7 @@
       </c>
       <c r="H291" s="5"/>
       <c r="I291" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="292" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -10494,7 +10508,7 @@
       </c>
       <c r="H292" s="5"/>
       <c r="I292" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="293" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -10517,7 +10531,7 @@
       </c>
       <c r="H293" s="5"/>
       <c r="I293" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="294" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -10542,7 +10556,7 @@
         <v>874</v>
       </c>
       <c r="I294" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="295" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -10567,7 +10581,7 @@
         <v>878</v>
       </c>
       <c r="I295" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="296" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -10590,7 +10604,7 @@
       </c>
       <c r="H296" s="5"/>
       <c r="I296" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="297" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -10613,7 +10627,7 @@
       </c>
       <c r="H297" s="5"/>
       <c r="I297" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="298" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -10636,7 +10650,7 @@
         <v>887</v>
       </c>
       <c r="I298" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="299" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -10659,7 +10673,7 @@
         <v>890</v>
       </c>
       <c r="I299" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="300" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -10682,7 +10696,7 @@
         <v>893</v>
       </c>
       <c r="I300" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="301" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -10705,7 +10719,7 @@
         <v>896</v>
       </c>
       <c r="I301" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="302" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -10725,7 +10739,7 @@
         <v>2</v>
       </c>
       <c r="I302" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="303" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -10748,7 +10762,7 @@
         <v>901</v>
       </c>
       <c r="I303" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="304" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -10771,7 +10785,7 @@
         <v>904</v>
       </c>
       <c r="I304" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="305" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -10794,7 +10808,7 @@
         <v>874</v>
       </c>
       <c r="I305" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="306" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -10817,7 +10831,7 @@
         <v>909</v>
       </c>
       <c r="I306" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="307" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -10840,7 +10854,7 @@
         <v>465</v>
       </c>
       <c r="I307" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="308" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -10863,7 +10877,7 @@
         <v>914</v>
       </c>
       <c r="I308" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="309" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -10886,7 +10900,7 @@
         <v>917</v>
       </c>
       <c r="I309" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="310" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -10906,7 +10920,7 @@
         <v>1</v>
       </c>
       <c r="I310" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="311" spans="1:9" ht="27" x14ac:dyDescent="0.2">
@@ -10929,7 +10943,7 @@
       </c>
       <c r="H311" s="8"/>
       <c r="I311" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="312" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -10952,7 +10966,7 @@
       </c>
       <c r="H312" s="5"/>
       <c r="I312" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="313" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -10975,7 +10989,7 @@
       </c>
       <c r="H313" s="5"/>
       <c r="I313" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="314" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -10998,7 +11012,7 @@
       </c>
       <c r="H314" s="5"/>
       <c r="I314" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="315" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -11021,7 +11035,7 @@
       </c>
       <c r="H315" s="5"/>
       <c r="I315" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="316" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -11044,7 +11058,7 @@
       </c>
       <c r="H316" s="5"/>
       <c r="I316" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="317" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -11067,7 +11081,7 @@
       </c>
       <c r="H317" s="8"/>
       <c r="I317" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="318" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -11090,7 +11104,7 @@
       </c>
       <c r="H318" s="5"/>
       <c r="I318" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="319" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -11113,7 +11127,7 @@
       </c>
       <c r="H319" s="5"/>
       <c r="I319" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="320" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -11136,7 +11150,7 @@
       </c>
       <c r="H320" s="5"/>
       <c r="I320" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="321" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -11159,7 +11173,7 @@
       </c>
       <c r="H321" s="5"/>
       <c r="I321" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="322" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -11182,7 +11196,7 @@
       </c>
       <c r="H322" s="8"/>
       <c r="I322" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="323" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -11205,7 +11219,7 @@
       </c>
       <c r="H323" s="5"/>
       <c r="I323" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="324" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -11228,7 +11242,7 @@
       </c>
       <c r="H324" s="5"/>
       <c r="I324" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="325" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -11251,7 +11265,7 @@
       </c>
       <c r="H325" s="5"/>
       <c r="I325" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="326" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -11274,7 +11288,7 @@
       </c>
       <c r="H326" s="5"/>
       <c r="I326" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="327" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -11297,7 +11311,7 @@
       </c>
       <c r="H327" s="5"/>
       <c r="I327" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="328" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -11322,7 +11336,7 @@
         <v>977</v>
       </c>
       <c r="I328" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="329" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -11345,7 +11359,7 @@
       </c>
       <c r="H329" s="5"/>
       <c r="I329" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="330" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -11370,7 +11384,7 @@
         <v>984</v>
       </c>
       <c r="I330" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="331" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -11395,7 +11409,7 @@
         <v>988</v>
       </c>
       <c r="I331" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="332" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -11418,7 +11432,7 @@
       </c>
       <c r="H332" s="5"/>
       <c r="I332" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="333" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -11441,7 +11455,7 @@
         <v>994</v>
       </c>
       <c r="I333" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="334" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -11464,7 +11478,7 @@
         <v>997</v>
       </c>
       <c r="I334" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="335" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -11484,7 +11498,7 @@
         <v>1</v>
       </c>
       <c r="I335" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="336" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -11504,7 +11518,7 @@
         <v>2</v>
       </c>
       <c r="I336" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="337" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -11524,7 +11538,7 @@
         <v>2</v>
       </c>
       <c r="I337" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="338" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -11544,7 +11558,7 @@
         <v>1</v>
       </c>
       <c r="I338" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="339" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -11567,7 +11581,7 @@
         <v>1008</v>
       </c>
       <c r="I339" s="1" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="340" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -11592,7 +11606,7 @@
       </c>
       <c r="H340" s="13"/>
       <c r="I340" s="1" t="s">
-        <v>1070</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="341" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -11619,7 +11633,7 @@
       </c>
       <c r="H341" s="13"/>
       <c r="I341" s="1" t="s">
-        <v>1070</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="342" spans="1:9" ht="53" x14ac:dyDescent="0.2">
@@ -11644,7 +11658,7 @@
       </c>
       <c r="H342" s="13"/>
       <c r="I342" s="1" t="s">
-        <v>1070</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="343" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -11669,7 +11683,7 @@
       </c>
       <c r="H343" s="13"/>
       <c r="I343" s="1" t="s">
-        <v>1070</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="344" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -11694,7 +11708,7 @@
       </c>
       <c r="H344" s="13"/>
       <c r="I344" s="1" t="s">
-        <v>1070</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="345" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -11717,7 +11731,7 @@
       </c>
       <c r="H345" s="13"/>
       <c r="I345" s="1" t="s">
-        <v>1070</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="346" spans="1:9" ht="66" x14ac:dyDescent="0.2">
@@ -11740,7 +11754,7 @@
       </c>
       <c r="H346" s="13"/>
       <c r="I346" s="1" t="s">
-        <v>1070</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="347" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -11767,7 +11781,7 @@
       </c>
       <c r="H347" s="13"/>
       <c r="I347" s="1" t="s">
-        <v>1070</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="348" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -11784,7 +11798,7 @@
         <v>0</v>
       </c>
       <c r="I348" s="1" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="349" spans="1:9" ht="105" x14ac:dyDescent="0.2">
@@ -11804,7 +11818,7 @@
         <v>0</v>
       </c>
       <c r="I349" s="1" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="350" spans="1:9" ht="144" x14ac:dyDescent="0.2">
@@ -11824,7 +11838,7 @@
         <v>0</v>
       </c>
       <c r="I350" s="1" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="351" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -11844,7 +11858,7 @@
         <v>0</v>
       </c>
       <c r="I351" s="1" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="352" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -11861,7 +11875,7 @@
         <v>0</v>
       </c>
       <c r="I352" s="1" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="353" spans="1:9" ht="79" x14ac:dyDescent="0.2">
@@ -11881,7 +11895,7 @@
         <v>0</v>
       </c>
       <c r="I353" s="1" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="354" spans="1:9" ht="157" x14ac:dyDescent="0.2">
@@ -11898,7 +11912,7 @@
         <v>0</v>
       </c>
       <c r="I354" s="1" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="355" spans="1:9" ht="183" x14ac:dyDescent="0.2">
@@ -11918,7 +11932,7 @@
         <v>0</v>
       </c>
       <c r="I355" s="1" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="356" spans="1:9" ht="92" x14ac:dyDescent="0.2">
@@ -11938,7 +11952,7 @@
         <v>0</v>
       </c>
       <c r="I356" s="1" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="357" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -11961,7 +11975,7 @@
         <v>0</v>
       </c>
       <c r="I357" s="1" t="s">
-        <v>1068</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="358" spans="1:9" ht="40" x14ac:dyDescent="0.2">
@@ -11984,13 +11998,61 @@
         <v>0</v>
       </c>
       <c r="I358" s="1" t="s">
-        <v>1068</v>
+        <v>1075</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <autoFilter ref="A1:I358" xr:uid="{2AB84084-35D3-FA4A-B5F4-F86FA41BD0A0}"/>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D263D798-6C76-254B-AE74-8D06E101C3D4}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>